<commit_message>
DRILL-7518: Support INT_64 for nullable INT64 in Parquet
closes #1952
</commit_message>
<xml_diff>
--- a/contrib/format-excel/src/test/resources/excel/test_data.xlsx
+++ b/contrib/format-excel/src/test/resources/excel/test_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cgivre/github/drill-dev/drill/contrib/format-excel/src/test/resources/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E97AF57-13DF-A343-AB5F-2E0128B9FC8B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0637A780-DC7A-1547-9037-6D4703C23137}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="54120" yWindow="7900" windowWidth="35260" windowHeight="20340" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="52280" yWindow="4120" windowWidth="35260" windowHeight="20340" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -20,13 +20,14 @@
     <sheet name="emptySheet" sheetId="6" r:id="rId5"/>
     <sheet name="missingDataSheet" sheetId="7" r:id="rId6"/>
     <sheet name="inconsistentData" sheetId="8" r:id="rId7"/>
+    <sheet name="comps" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="78">
   <si>
     <t>id</t>
   </si>
@@ -191,20 +192,98 @@
   </si>
   <si>
     <t>Anne</t>
+  </si>
+  <si>
+    <t>Close Date</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Style</t>
+  </si>
+  <si>
+    <t>Beds</t>
+  </si>
+  <si>
+    <t>Full Bath</t>
+  </si>
+  <si>
+    <t>Half Bath</t>
+  </si>
+  <si>
+    <t>Sq Footage</t>
+  </si>
+  <si>
+    <t>List Price</t>
+  </si>
+  <si>
+    <t>Close Price</t>
+  </si>
+  <si>
+    <t>Days on Market</t>
+  </si>
+  <si>
+    <t>Asking - Sold Delta Percent</t>
+  </si>
+  <si>
+    <t>Price per sq. foot</t>
+  </si>
+  <si>
+    <t>Hi Rise</t>
+  </si>
+  <si>
+    <t>Contemporary</t>
+  </si>
+  <si>
+    <t>Detached</t>
+  </si>
+  <si>
+    <t>Split Level</t>
+  </si>
+  <si>
+    <t>Colonial</t>
+  </si>
+  <si>
+    <t>Rancher</t>
+  </si>
+  <si>
+    <t>Cape Cod</t>
+  </si>
+  <si>
+    <t>Traditional</t>
+  </si>
+  <si>
+    <t>French Country</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Townhouse</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Arial"/>
       <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -227,9 +306,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -915,7 +1001,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EB87CDA-D288-6140-983A-9CBE9D71D9D4}">
   <dimension ref="A3:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
+    <sheetView showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
@@ -1141,4 +1227,580 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E4F5EFA-37CF-6F4E-9599-85DA98E59077}">
+  <dimension ref="A1:L14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A2" s="5">
+        <v>41915</v>
+      </c>
+      <c r="B2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>3750</v>
+      </c>
+      <c r="H2">
+        <v>400000</v>
+      </c>
+      <c r="I2">
+        <v>385000</v>
+      </c>
+      <c r="J2">
+        <v>15</v>
+      </c>
+      <c r="K2" s="6">
+        <f>I2/H2</f>
+        <v>0.96250000000000002</v>
+      </c>
+      <c r="L2" s="7">
+        <f>I2/G2</f>
+        <v>102.66666666666667</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A3" s="5">
+        <v>41919</v>
+      </c>
+      <c r="B3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>1957</v>
+      </c>
+      <c r="H3">
+        <v>315000</v>
+      </c>
+      <c r="I3">
+        <v>285000</v>
+      </c>
+      <c r="J3">
+        <v>142</v>
+      </c>
+      <c r="K3" s="6">
+        <f t="shared" ref="K3:K14" si="0">I3/H3</f>
+        <v>0.90476190476190477</v>
+      </c>
+      <c r="L3" s="7">
+        <f t="shared" ref="L3:L14" si="1">I3/G3</f>
+        <v>145.63106796116506</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A4" s="5">
+        <v>41932</v>
+      </c>
+      <c r="B4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>2536</v>
+      </c>
+      <c r="H4">
+        <v>246000</v>
+      </c>
+      <c r="I4">
+        <v>275000</v>
+      </c>
+      <c r="J4">
+        <v>8</v>
+      </c>
+      <c r="K4" s="6">
+        <f t="shared" si="0"/>
+        <v>1.1178861788617886</v>
+      </c>
+      <c r="L4" s="7">
+        <f t="shared" si="1"/>
+        <v>108.4384858044164</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A5" s="5">
+        <v>41953</v>
+      </c>
+      <c r="B5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>1728</v>
+      </c>
+      <c r="H5">
+        <v>350000</v>
+      </c>
+      <c r="I5">
+        <v>336000</v>
+      </c>
+      <c r="J5">
+        <v>14</v>
+      </c>
+      <c r="K5" s="6">
+        <f t="shared" si="0"/>
+        <v>0.96</v>
+      </c>
+      <c r="L5" s="7">
+        <f t="shared" si="1"/>
+        <v>194.44444444444446</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A6" s="5">
+        <v>41976</v>
+      </c>
+      <c r="B6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>2034</v>
+      </c>
+      <c r="H6">
+        <v>449800</v>
+      </c>
+      <c r="I6">
+        <v>375000</v>
+      </c>
+      <c r="J6">
+        <v>106</v>
+      </c>
+      <c r="K6" s="6">
+        <f t="shared" si="0"/>
+        <v>0.83370386838594934</v>
+      </c>
+      <c r="L6" s="7">
+        <f t="shared" si="1"/>
+        <v>184.36578171091446</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A7" s="5">
+        <v>41978</v>
+      </c>
+      <c r="B7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" t="s">
+        <v>74</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>3110</v>
+      </c>
+      <c r="H7">
+        <v>649700</v>
+      </c>
+      <c r="I7">
+        <v>527601</v>
+      </c>
+      <c r="J7">
+        <v>231</v>
+      </c>
+      <c r="K7" s="6">
+        <f t="shared" si="0"/>
+        <v>0.81206864706787751</v>
+      </c>
+      <c r="L7" s="7">
+        <f t="shared" si="1"/>
+        <v>169.64662379421222</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A8" s="5">
+        <v>41978</v>
+      </c>
+      <c r="B8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>2137</v>
+      </c>
+      <c r="H8">
+        <v>499000</v>
+      </c>
+      <c r="I8">
+        <v>375000</v>
+      </c>
+      <c r="J8">
+        <v>140</v>
+      </c>
+      <c r="K8" s="6">
+        <f t="shared" si="0"/>
+        <v>0.75150300601202402</v>
+      </c>
+      <c r="L8" s="7">
+        <f t="shared" si="1"/>
+        <v>175.47964436125409</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A9" s="5">
+        <v>41988</v>
+      </c>
+      <c r="B9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D9">
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>2766</v>
+      </c>
+      <c r="H9">
+        <v>549000</v>
+      </c>
+      <c r="I9">
+        <v>507500</v>
+      </c>
+      <c r="J9">
+        <v>85</v>
+      </c>
+      <c r="K9" s="6">
+        <f t="shared" si="0"/>
+        <v>0.92440801457194899</v>
+      </c>
+      <c r="L9" s="7">
+        <f t="shared" si="1"/>
+        <v>183.47794649313087</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A10" s="5">
+        <v>42002</v>
+      </c>
+      <c r="B10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>2716</v>
+      </c>
+      <c r="H10">
+        <v>469000</v>
+      </c>
+      <c r="I10">
+        <v>425000</v>
+      </c>
+      <c r="J10">
+        <v>26</v>
+      </c>
+      <c r="K10" s="6">
+        <f t="shared" si="0"/>
+        <v>0.906183368869936</v>
+      </c>
+      <c r="L10" s="7">
+        <f t="shared" si="1"/>
+        <v>156.48011782032401</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A11" s="5">
+        <v>42002</v>
+      </c>
+      <c r="B11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11">
+        <v>3</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1444</v>
+      </c>
+      <c r="H11">
+        <v>154900</v>
+      </c>
+      <c r="I11">
+        <v>154900</v>
+      </c>
+      <c r="J11">
+        <v>9</v>
+      </c>
+      <c r="K11" s="6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L11" s="7">
+        <f t="shared" si="1"/>
+        <v>107.27146814404432</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A12" s="5">
+        <v>42004</v>
+      </c>
+      <c r="B12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D12">
+        <v>6</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>1152</v>
+      </c>
+      <c r="H12">
+        <v>339000</v>
+      </c>
+      <c r="I12">
+        <v>339000</v>
+      </c>
+      <c r="J12">
+        <v>107</v>
+      </c>
+      <c r="K12" s="6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L12" s="7">
+        <f t="shared" si="1"/>
+        <v>294.27083333333331</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A13" s="5">
+        <v>42010</v>
+      </c>
+      <c r="B13" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" t="s">
+        <v>73</v>
+      </c>
+      <c r="D13">
+        <v>4</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>1592</v>
+      </c>
+      <c r="H13">
+        <v>220000</v>
+      </c>
+      <c r="I13">
+        <v>201000</v>
+      </c>
+      <c r="J13">
+        <v>43</v>
+      </c>
+      <c r="K13" s="6">
+        <f t="shared" si="0"/>
+        <v>0.91363636363636369</v>
+      </c>
+      <c r="L13" s="7">
+        <f t="shared" si="1"/>
+        <v>126.25628140703517</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A14" s="5">
+        <v>42019</v>
+      </c>
+      <c r="B14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" t="s">
+        <v>70</v>
+      </c>
+      <c r="D14">
+        <v>4</v>
+      </c>
+      <c r="E14">
+        <v>3</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>1957</v>
+      </c>
+      <c r="H14">
+        <v>385500</v>
+      </c>
+      <c r="I14">
+        <v>370000</v>
+      </c>
+      <c r="J14">
+        <v>11</v>
+      </c>
+      <c r="K14" s="6">
+        <f t="shared" si="0"/>
+        <v>0.95979247730220496</v>
+      </c>
+      <c r="L14" s="7">
+        <f t="shared" si="1"/>
+        <v>189.0648952478283</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
DRILL-7723: Add Excel Metadata as Implicit Fields
</commit_message>
<xml_diff>
--- a/contrib/format-excel/src/test/resources/excel/test_data.xlsx
+++ b/contrib/format-excel/src/test/resources/excel/test_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cgivre/github/drill-dev/drill/contrib/format-excel/src/test/resources/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0637A780-DC7A-1547-9037-6D4703C23137}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D24C478-BB41-CB4D-817A-62FC5708BA64}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="52280" yWindow="4120" windowWidth="35260" windowHeight="20340" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>

<commit_message>
DRILL-8006: Leading and Trailing Whitespace Causes Query Failures in Excel Files (#2325)
* Initial Commit

* Delete logback-test.xml
</commit_message>
<xml_diff>
--- a/contrib/format-excel/src/test/resources/excel/test_data.xlsx
+++ b/contrib/format-excel/src/test/resources/excel/test_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cgivre/github/drill-dev/drill/contrib/format-excel/src/test/resources/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D24C478-BB41-CB4D-817A-62FC5708BA64}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD9D6CE3-7B29-CE42-AFAB-CCF8E419C8EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="52280" yWindow="4120" windowWidth="35260" windowHeight="20340" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="52280" yWindow="4120" windowWidth="35260" windowHeight="20340" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -21,13 +21,25 @@
     <sheet name="missingDataSheet" sheetId="7" r:id="rId6"/>
     <sheet name="inconsistentData" sheetId="8" r:id="rId7"/>
     <sheet name="comps" sheetId="9" r:id="rId8"/>
+    <sheet name="spaceInColHeader" sheetId="10" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="79">
   <si>
     <t>id</t>
   </si>
@@ -261,6 +273,9 @@
   </si>
   <si>
     <t>Townhouse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">col2 </t>
   </si>
 </sst>
 </file>
@@ -1233,7 +1248,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E4F5EFA-37CF-6F4E-9599-85DA98E59077}">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
@@ -1803,4 +1818,43 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2239CDA4-D7E0-0845-8071-70A4E440723B}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>